<commit_message>
docs: bills and docs updated
</commit_message>
<xml_diff>
--- a/bills/Bills.xlsx
+++ b/bills/Bills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\dhonan-ubuntu\Workspaces\TankScope\bills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788F8556-33D9-4AA5-9D9C-976CC462AB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96684F7-17BA-4603-8A53-FD7965C4E721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>No</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Cadangan Saklar + Resistor</t>
+  </si>
+  <si>
+    <t>Wing Bolt</t>
+  </si>
+  <si>
+    <t>Rubber Pad</t>
   </si>
 </sst>
 </file>
@@ -245,12 +251,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -259,6 +259,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,10 +582,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -591,14 +597,14 @@
       <c r="E2" s="4">
         <v>59523.66</v>
       </c>
-      <c r="F2" s="8">
-        <f>SUM(E2:E34)</f>
-        <v>1706474.1600000001</v>
+      <c r="F2" s="6">
+        <f>SUM(E2:E36)</f>
+        <v>1739774.1600000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
@@ -608,11 +614,11 @@
       <c r="E3" s="4">
         <v>393021.5</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
@@ -622,11 +628,11 @@
       <c r="E4" s="4">
         <v>27824</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
@@ -636,13 +642,13 @@
       <c r="E5" s="4">
         <v>74588</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -654,11 +660,11 @@
       <c r="E6" s="4">
         <v>19750</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
@@ -668,11 +674,11 @@
       <c r="E7" s="4">
         <v>29110</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
@@ -682,55 +688,55 @@
       <c r="E8" s="4">
         <v>651850</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="9">
         <v>11</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="10">
         <v>62490</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
@@ -740,45 +746,45 @@
       <c r="E13" s="4">
         <v>48400</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="9">
         <v>13</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="10">
         <v>34800</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="3" t="s">
         <v>31</v>
       </c>
@@ -788,35 +794,35 @@
       <c r="E17" s="4">
         <v>67000</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="9">
         <v>15</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="10">
         <v>31845</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="3" t="s">
         <v>27</v>
       </c>
@@ -826,11 +832,11 @@
       <c r="E20" s="4">
         <v>44100</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="3" t="s">
         <v>38</v>
       </c>
@@ -840,77 +846,99 @@
       <c r="E21" s="4">
         <v>17400</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2">
+        <v>21</v>
+      </c>
+      <c r="E22" s="4">
+        <v>17200</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="2">
+        <v>22</v>
+      </c>
+      <c r="E23" s="4">
+        <v>13100</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="5">
-        <v>7000</v>
-      </c>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="E24" s="5">
+        <v>10000</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>3</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B25" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D25" s="2">
         <v>17</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E25" s="5">
         <v>13700</v>
       </c>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="3" t="s">
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D26" s="2">
         <v>19</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E26" s="5">
         <v>10500</v>
       </c>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>4</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D27" s="2">
         <v>18</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E27" s="5">
         <v>113572</v>
       </c>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E27" s="1"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="1"/>
@@ -918,21 +946,27 @@
     <row r="29" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F2:F25"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
     <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B22"/>
+    <mergeCell ref="B6:B24"/>
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A22"/>
+    <mergeCell ref="A6:A24"/>
     <mergeCell ref="E9:E12"/>
     <mergeCell ref="D9:D12"/>
     <mergeCell ref="D14:D16"/>

</xml_diff>